<commit_message>
TP 8 casi terminado
</commit_message>
<xml_diff>
--- a/TP 8/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/TP 8/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Ingenieria de software ll\ing-sw-II\TP 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F21B46-CB8D-407A-9FF8-242789597916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBA139A-93D8-4EFE-838A-AC9DDB93B9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="6384" windowWidth="5328" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -254,7 +254,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +553,7 @@
       </c>
       <c r="C2">
         <f>ROUND(C24,0)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -562,7 +562,7 @@
       </c>
       <c r="C3">
         <f>ROUND(C25,0)</f>
-        <v>98</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -606,15 +606,15 @@
       </c>
       <c r="E5" s="6">
         <f>$C$24*EXP($C$23*A5)</f>
-        <v>11.289858321662283</v>
+        <v>16.314987271867508</v>
       </c>
       <c r="F5" s="9">
         <f>ROUND(E5,0)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G5" s="9">
         <f>F5</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -635,15 +635,15 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" ref="E6:E21" si="1">$C$24*EXP($C$23*A6)</f>
-        <v>10.062771424865511</v>
+        <v>12.160967691664849</v>
       </c>
       <c r="F6" s="9">
-        <f t="shared" ref="F6:F16" si="2">ROUND(E6,0)</f>
-        <v>10</v>
+        <f t="shared" ref="F6:F21" si="2">ROUND(E6,0)</f>
+        <v>12</v>
       </c>
       <c r="G6" s="9">
         <f>G5+F6</f>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -664,7 +664,7 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>8.9690557546501424</v>
+        <v>9.0646184844242317</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="2"/>
@@ -672,7 +672,7 @@
       </c>
       <c r="G7" s="9">
         <f t="shared" ref="G7:G21" si="4">G6+F7</f>
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -693,15 +693,15 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>7.9942152845927286</v>
+        <v>6.7566422633030339</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -722,15 +722,15 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>7.1253295513613226</v>
+        <v>5.0363084505649205</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -746,20 +746,20 @@
         <v>64</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10:D11" si="6">IF(B10&gt;0,LN(B10),0)</f>
+        <f t="shared" ref="D10:D21" si="6">IF(B10&gt;0,LN(B10),0)</f>
         <v>0.69314718055994529</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>6.3508824078521791</v>
+        <v>3.7539952273323505</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,15 +780,15 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>5.6606093890296441</v>
+        <v>2.7981765424342329</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="4"/>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -796,17 +796,21 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
+      <c r="D12" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>5.0453616674674189</v>
+        <v>2.0857224073226059</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -814,17 +818,21 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
+      <c r="D13" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="E13" s="6">
         <f t="shared" si="1"/>
-        <v>4.4969847954679816</v>
+        <v>1.5546688689710686</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,17 +840,21 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
+      <c r="D14" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="E14" s="6">
         <f t="shared" si="1"/>
-        <v>4.0082106266172444</v>
+        <v>1.1588288468600301</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -850,17 +862,21 @@
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
+      <c r="D15" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>3.5725609843107122</v>
+        <v>0.86377512479793417</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15" s="9">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -870,106 +886,149 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" si="1"/>
-        <v>3.184261800480956</v>
+        <v>0.643846128133023</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" si="4"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="1"/>
-        <v>2.8381665865274321</v>
-      </c>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.47991407116390322</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="1"/>
-        <v>2.5296882221380508</v>
-      </c>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.35772136483754219</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="1"/>
-        <v>2.2547381579365648</v>
-      </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.26664059786971883</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="1"/>
-        <v>2.0096722261521989</v>
-      </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.19875024368368274</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="1"/>
-        <v>1.7912423410901275</v>
-      </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.1481457050423502</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="H21" s="9">
+        <f>G21*0.9</f>
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="7">
         <f>INTERCEPT(D5:D21,A5:A21)</f>
-        <v>2.4239048290715188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2.7920841498958842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="7">
         <f>SLOPE(D5:D21,A5:A21)</f>
-        <v>-0.11506221279094787</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-0.29385269661752728</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24">
         <f>EXP(C22)</f>
-        <v>11.289858321662283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16.314987271867508</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C25">
         <f>-C24/C23</f>
-        <v>98.11960023899762</v>
+        <v>55.520971764648344</v>
+      </c>
+      <c r="D25">
+        <f>ROUND(C25,0)</f>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>